<commit_message>
Registro y cargue de anotaciones en flipbook
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/09_formato_cargue_programas.xlsx
+++ b/assets/formatos_cargue/09_formato_cargue_programas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\editores\assets\formatos_cargue\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">programas!$A$1:$E$485</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -23,7 +28,7 @@
     <author>Mauricio</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,6 +120,30 @@
           </rPr>
           <t xml:space="preserve">
 Código de la institución, número que aparece en el listado de instituciones de la plataforma.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Pacarina:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cantidad de unidades en las que se divide el programa</t>
         </r>
       </text>
     </comment>
@@ -128,7 +157,7 @@
     <author>Mauricio</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>nivel</t>
   </si>
@@ -243,13 +272,34 @@
   </si>
   <si>
     <t>código área</t>
+  </si>
+  <si>
+    <t>Cantidad unidades</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>Competencias Ciudadanas</t>
+  </si>
+  <si>
+    <t>Inglés</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>otr</t>
+  </si>
+  <si>
+    <t>Otras áreas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +327,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -365,12 +428,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -412,7 +478,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,7 +513,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -663,7 +729,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="5" customWidth="1"/>
@@ -694,7 +760,9 @@
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -716,6 +784,9 @@
       <c r="E2" s="3">
         <v>41</v>
       </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -733,6 +804,9 @@
       <c r="E3" s="3">
         <v>41</v>
       </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -750,6 +824,9 @@
       <c r="E4" s="3">
         <v>41</v>
       </c>
+      <c r="F4" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -766,6 +843,9 @@
       </c>
       <c r="E5" s="3">
         <v>41</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -777,13 +857,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
@@ -843,6 +923,30 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>